<commit_message>
Updating dev shortcuts to goto github repos now
</commit_message>
<xml_diff>
--- a/MicrosoftErgonomicKeyboardTemplate.xlsx
+++ b/MicrosoftErgonomicKeyboardTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PChenry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,12 +60,6 @@
     <t>Next</t>
   </si>
   <si>
-    <t>Dev</t>
-  </si>
-  <si>
-    <t>Docs</t>
-  </si>
-  <si>
     <t>Mute</t>
   </si>
   <si>
@@ -73,6 +67,14 @@
   </si>
   <si>
     <t>Vol+</t>
+  </si>
+  <si>
+    <t>GitHub\
+PCHenry</t>
+  </si>
+  <si>
+    <t>GitHub\
+Victanya</t>
   </si>
 </sst>
 </file>
@@ -291,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -343,6 +345,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,7 +386,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E81275FA-B807-45D0-95BA-B3028F00F66E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E81275FA-B807-45D0-95BA-B3028F00F66E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -442,7 +447,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67DADC1F-4FCE-4127-8ABC-DDE558106780}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DADC1F-4FCE-4127-8ABC-DDE558106780}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -486,7 +491,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0C7B0966-8AC7-4D01-895A-848816EBEC1C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C7B0966-8AC7-4D01-895A-848816EBEC1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -530,7 +535,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6A80ACB3-109F-4E48-A35B-61BB3A3E0534}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A80ACB3-109F-4E48-A35B-61BB3A3E0534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -569,7 +574,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -608,7 +613,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -647,7 +652,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1166,7 +1171,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,22 +1221,22 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
+      <c r="I2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Adding new chrome profile and removing one github shortcut
</commit_message>
<xml_diff>
--- a/MicrosoftErgonomicKeyboardTemplate.xlsx
+++ b/MicrosoftErgonomicKeyboardTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PChenry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PCHenry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -69,12 +69,10 @@
     <t>Vol+</t>
   </si>
   <si>
-    <t>GitHub\
-PCHenry</t>
+    <t>GitHub</t>
   </si>
   <si>
-    <t>GitHub\
-Victanya</t>
+    <t>Dev</t>
   </si>
 </sst>
 </file>
@@ -386,7 +384,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E81275FA-B807-45D0-95BA-B3028F00F66E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E81275FA-B807-45D0-95BA-B3028F00F66E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -447,7 +445,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DADC1F-4FCE-4127-8ABC-DDE558106780}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67DADC1F-4FCE-4127-8ABC-DDE558106780}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -491,7 +489,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C7B0966-8AC7-4D01-895A-848816EBEC1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0C7B0966-8AC7-4D01-895A-848816EBEC1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -535,7 +533,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A80ACB3-109F-4E48-A35B-61BB3A3E0534}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6A80ACB3-109F-4E48-A35B-61BB3A3E0534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -574,7 +572,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -602,45 +600,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="409575" cy="493610"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5219699" y="657225"/>
-          <a:ext cx="409575" cy="493610"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -652,7 +611,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65186B20-B5C5-45B0-BB97-F93092742A0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -860,6 +819,44 @@
         <a:xfrm>
           <a:off x="3510645" y="762002"/>
           <a:ext cx="328658" cy="266737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>560614</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>647701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5078185" y="664029"/>
+          <a:ext cx="538843" cy="538843"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1171,7 +1168,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,10 +1230,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>12</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>1</v>

</xml_diff>